<commit_message>
Fixed standard curve files 2023_12_21
 - fixed standard curve files values to correct version
</commit_message>
<xml_diff>
--- a/gx_stdcurves/GXWW_stdcurves_2023_12_21.xlsx
+++ b/gx_stdcurves/GXWW_stdcurves_2023_12_21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://022gc.sharepoint.com/sites/Communicablediseasesandinfectioncontrol-ScienceandTechnol426/Shared Documents/Wastewater/GX github files/gx_stdcurves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{3F59A943-59C7-4F91-ADF8-A1DCF37287E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{043A234F-E55C-4EE2-952F-921EDB8D3625}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{3F59A943-59C7-4F91-ADF8-A1DCF37287E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2D43F73-CD8B-4605-B8AE-32FFE5DAA54E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3E8043DA-D2AD-46AB-BEA9-6CBF79AEE5DC}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{3E8043DA-D2AD-46AB-BEA9-6CBF79AEE5DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
         <v>-3.2069999999999999</v>
       </c>
       <c r="D2" s="2">
-        <v>42.433999999999997</v>
+        <v>43.146000000000001</v>
       </c>
       <c r="E2" s="3">
         <v>1.05</v>
@@ -529,7 +529,7 @@
         <v>-3.4790000000000001</v>
       </c>
       <c r="D3" s="2">
-        <v>43.146000000000001</v>
+        <v>43.487000000000002</v>
       </c>
       <c r="E3" s="3">
         <v>0.93799999999999994</v>
@@ -648,26 +648,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC70BFA850CCAE47A7BAA0F38D9D36E7" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d79f54030d35a05c2837f0b87c130511">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ab521e1-8720-4533-8025-5c945dd49c24" xmlns:ns3="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94f9cccdc7784000b8a29c3f81994f46" ns2:_="" ns3:_="">
     <xsd:import namespace="4ab521e1-8720-4533-8025-5c945dd49c24"/>
@@ -890,26 +870,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7FC959E-0488-43DB-BB68-A9417058EC21}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
-    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F26B313E-8105-4C95-AE0C-DE3995CD9D4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CABC56D1-873D-4797-868C-76C56824B78A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -926,4 +907,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F26B313E-8105-4C95-AE0C-DE3995CD9D4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7FC959E-0488-43DB-BB68-A9417058EC21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
+    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>